<commit_message>
Server ParkingLot 문서 변경
</commit_message>
<xml_diff>
--- a/DesignDocument/(5Team_Design_001) Interface description document.xlsx
+++ b/DesignDocument/(5Team_Design_001) Interface description document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\surepark\SureParkSystem\DesignDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Now\CMU\SureParkSystem\DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838"/>
+    <workbookView xWindow="9840" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parkinglot→ParkServer" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,20 +165,6 @@
   </si>
   <si>
     <t>messagetype (string)
-led_number (int)
-status (string)
-timestamp (int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>messagetype (string)
-sensor_number (int)
-status (string)
-timestamp (int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>messagetype (string)
 id (string)
 pwd (string)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,20 +193,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"messagetype" : "Parkingslot_LED",
-"sendor_number" : 2,
-"status" : "off",
-"timestamp" : 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"messagetype" : "Parkingslot_Sensor",
-"sendor_number" : 2,
-"status" : "empty",
-"timestamp" : 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"messagetype" : "ExitGate_LED",
 "status" : "red",
 "timestamp" : 60</t>
@@ -281,12 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"messagetype" : "Parkingslot_LED",
-"sensor_number" : 3,
-"command" : "on"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>messagetype (string)
 result (string)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,12 +260,6 @@
   <si>
     <t>messagetype (string)
 command (string)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>messagetype (string)
-sensor_number (int)
-status (string)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -526,34 +486,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>messagetype (string)
-slot_number (int)
-slot_status (string[])
-led_status (string[])
-entrygate (string)
-exitgate (string)
-entrygateled (string)
-exitgateled (string)
-entrygate_arrive (string)
-exitgate_arrive (string)
-timestamp (int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"messagetype" : "Parkinglot_Information",
-"slot_number" : 4,
-"slot_status" : {"1", "1", "0", "1"},
-"led_status" : {"0", "0", "0", "0"},
-"entrygate" : "0",
-"exitgate" : "0",
-"entrygateled" : "0",
-"exitgateled" : "1",
-"entrygate_arrive" : "0",
-"exitgate_arrive" : "0",
-"timestamp" : 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">
 1~10
 empty or occupied
@@ -567,12 +499,248 @@
 -</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">messagetype (string)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (int)
+status (string)
+timestamp (int)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"messagetype" : "Parkingslot_Sensor",
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : 2,
+"status" : "empty",
+"timestamp" : 10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"messagetype" : "Parkingslot_LED",
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : 2,
+"status" : "off",
+"timestamp" : 15</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">messagetype (string)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (int)
+slot_status (string[])
+led_status (string[])
+entrygate (string)
+exitgate (string)
+entrygateled (string)
+exitgateled (string)
+entrygate_arrive (string)
+exitgate_arrive (string)
+timestamp (int)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"messagetype" : "Parkinglot_Information",
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : 4,
+"slot_status" : {"1", "1", "0", "1"},
+"led_status" : {"0", "0", "0", "0"},
+"entrygate" : "0",
+"exitgate" : "0",
+"entrygateled" : "0",
+"exitgateled" : "1",
+"entrygate_arrive" : "0",
+"exitgate_arrive" : "0",
+"timestamp" : 5</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">messagetype (string)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (int)
+status (string)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"messagetype" : "Parkingslot_LED",
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : 3,
+"command" : "on"</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +760,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -983,11 +1160,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1026,7 +1203,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -1043,16 +1220,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="66" x14ac:dyDescent="0.3">
@@ -1063,13 +1240,13 @@
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="66" x14ac:dyDescent="0.3">
@@ -1080,13 +1257,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -1103,7 +1280,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -1120,7 +1297,7 @@
         <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -1137,7 +1314,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -1154,7 +1331,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1165,13 +1342,13 @@
         <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1182,13 +1359,13 @@
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1199,13 +1376,13 @@
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1216,13 +1393,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1233,13 +1410,13 @@
         <v>23</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1253,11 +1430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1295,13 +1472,13 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1312,13 +1489,13 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1329,13 +1506,13 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1346,13 +1523,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1363,13 +1540,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -1380,13 +1557,13 @@
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1397,13 +1574,13 @@
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1459,7 +1636,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -1473,16 +1650,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1493,13 +1670,13 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1555,13 +1732,13 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
@@ -1569,16 +1746,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
@@ -1586,19 +1763,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1653,7 +1830,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -1667,16 +1844,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="99" x14ac:dyDescent="0.3">
@@ -1684,16 +1861,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -1701,16 +1878,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="66" x14ac:dyDescent="0.3">
@@ -1718,16 +1895,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1783,13 +1960,13 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="181.5" x14ac:dyDescent="0.3">
@@ -1797,16 +1974,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="66" x14ac:dyDescent="0.3">
@@ -1814,19 +1991,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="115.5" x14ac:dyDescent="0.3">
@@ -1834,16 +2011,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ParkServer <--> ParkingLot 메시지 추가(Reset)
</commit_message>
<xml_diff>
--- a/DesignDocument/(5Team_Design_001) Interface description document.xlsx
+++ b/DesignDocument/(5Team_Design_001) Interface description document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\surepark\SureParkSystem\DesignDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Now\CMU\SureParkSystem\DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23280" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="23280" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838"/>
   </bookViews>
   <sheets>
     <sheet name="Parkinglot→ParkServer" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -348,172 +348,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">messagetype (string)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (int)
-status (string)
-timestamp (int)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"messagetype" : "Parkingslot_Sensor",
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : 2,
-"status" : "empty",
-"timestamp" : 10</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"messagetype" : "Parkingslot_LED",
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : 2,
-"status" : "off",
-"timestamp" : 15</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">messagetype (string)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_count</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (int)
-slot_status (string[])
-led_status (string[])
-entrygate (string)
-exitgate (string)
-entrygateled (string)
-exitgateled (string)
-entrygate_arrive (string)
-exitgate_arrive (string)
-timestamp (int)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"messagetype" : "Parkingslot_LED",
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : 3,
-"command" : "on"</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>messagetype (string)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -594,45 +428,6 @@
 "graceperiod" : "120",
 "paymentinfo" : "2222333344445555",
 "configrmationinfo" : "sanghee, aabbccdd"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"messagetype" : "Parkinglot_Information",
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_count</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : 4,
-"slot_status" : ["1", "1", "0", "1"],
-"led_status" : ["0", "0", "0", "0"],
-"entrygate" : "0",
-"exitgate" : "0",
-"entrygateled" : "0",
-"exitgateled" : "1",
-"entrygate_arrive" : "0",
-"exitgate_arrive" : "0",
-"timestamp" : 5</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1237,37 +1032,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">messagetype (string)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slot_number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (int)
-command (string)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">
 1~10
 on or off</t>
@@ -1361,12 +1125,94 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"messagetype" : "Reset",
+"timestamp" : 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">messagetype (string)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slot_number (int)
+command (string)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"messagetype" : "Parkingslot_LED",
+"slot_number" : 3,
+"command" : "on"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>messagetype (string)
+slot_count (int)
+slot_status (string[])
+led_status (string[])
+entrygate (string)
+exitgate (string)
+entrygateled (string)
+exitgateled (string)
+entrygate_arrive (string)
+exitgate_arrive (string)
+timestamp (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"messagetype" : "Parkinglot_Information",
+"slot_count" : 4,
+"slot_status" : ["1", "1", "0", "1"],
+"led_status" : ["0", "0", "0", "0"],
+"entrygate" : "0",
+"exitgate" : "0",
+"entrygateled" : "0",
+"exitgateled" : "1",
+"entrygate_arrive" : "0",
+"exitgate_arrive" : "0",
+"timestamp" : 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>messagetype (string)
+slot_number (int)
+status (string)
+timestamp (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"messagetype" : "Parkingslot_Sensor",
+"slot_number" : 2,
+"status" : "empty",
+"timestamp" : 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"messagetype" : "Parkingslot_LED",
+"slot_number" : 2,
+"status" : "off",
+"timestamp" : 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1392,15 +1238,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
@@ -1413,6 +1250,20 @@
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -1471,7 +1322,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1496,22 +1347,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1820,14 +1680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -1838,7 +1698,7 @@
     <col min="7" max="7" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1855,7 +1715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1872,61 +1732,61 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="181.5">
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>83</v>
+      <c r="F4" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="66">
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="F5" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="66">
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="F6" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="49.5">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1943,7 +1803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="49.5">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1960,7 +1820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="49.5">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1977,7 +1837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="49.5">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1994,7 +1854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="33" customHeight="1">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -2011,7 +1871,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="33" customHeight="1">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -2028,7 +1888,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="33" customHeight="1">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -2045,7 +1905,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="33" customHeight="1">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -2062,7 +1922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="33" customHeight="1">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -2098,7 +1958,7 @@
       <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2109,7 +1969,7 @@
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +1986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="33">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2143,55 +2003,55 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="49.5">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>29</v>
@@ -2206,16 +2066,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2225,7 +2085,7 @@
     <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="33" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="33" customHeight="1">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2259,7 +2119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="33" customHeight="1">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2276,7 +2136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="33" customHeight="1">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2293,12 +2153,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="33" customHeight="1">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>51</v>
@@ -2310,12 +2170,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="33" customHeight="1">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>51</v>
@@ -2327,24 +2187,24 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="49.5">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="33" customHeight="1">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -2359,6 +2219,23 @@
       </c>
       <c r="F9" s="3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="33">
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2379,7 +2256,7 @@
       <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2389,7 +2266,7 @@
     <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2423,7 +2300,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2431,13 +2308,13 @@
         <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2457,7 +2334,7 @@
       <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2468,7 +2345,7 @@
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2485,7 +2362,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2493,16 +2370,16 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="99" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="99">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -2510,16 +2387,16 @@
         <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="49.5">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2558,7 +2435,7 @@
       <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2568,7 +2445,7 @@
     <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2585,7 +2462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2602,7 +2479,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2610,16 +2487,16 @@
         <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="82.5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="82.5">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2627,16 +2504,16 @@
         <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="33">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2644,16 +2521,16 @@
         <v>62</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="49.5">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -2661,30 +2538,30 @@
         <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="66">
       <c r="B8" s="12">
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +2583,7 @@
       <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2717,7 +2594,7 @@
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2734,7 +2611,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2742,33 +2619,33 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="99" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="99">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="165" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="165">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2776,33 +2653,33 @@
         <v>63</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="49.5">
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2824,7 +2701,7 @@
       <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -2834,7 +2711,7 @@
     <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2851,7 +2728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2868,7 +2745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2876,131 +2753,131 @@
         <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="49.5">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="49.5">
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="49.5">
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="82.5">
       <c r="B8" s="2">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="33">
       <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="99" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="99">
       <c r="B10" s="2">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="33">
       <c r="B11" s="2">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3014,15 +2891,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -3033,7 +2910,7 @@
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3050,7 +2927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -3058,64 +2935,64 @@
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="99" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="99">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="165" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="165">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="66">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -3138,7 +3015,7 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="2" width="5.75" customWidth="1"/>
@@ -3148,7 +3025,7 @@
     <col min="6" max="6" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="33" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3165,7 +3042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="49.5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -3182,24 +3059,24 @@
         <v>31</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="33">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graceperiod_list (string[]) parking_fee_list (string[]) parkinglot_id_list (string[]) parkinglot_location_list (string[]) 인터페이스 문서 변경
</commit_message>
<xml_diff>
--- a/DesignDocument/(5Team_Design_001) Interface description document.xlsx
+++ b/DesignDocument/(5Team_Design_001) Interface description document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\surepark\SureParkSystem\DesignDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Now\CMU\SureParkSystem\DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="24240" yWindow="30" windowWidth="21555" windowHeight="10305" tabRatio="838" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parkinglot→ParkServer" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="146">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -796,88 +796,6 @@
     <t>"messagetype" : "Authentication_Response",
 "result" : "ok",
 "authority" : 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>messagetype (string)
-parkinglot_count (int)
-parkinglot_id (string[])
-parkinglot_location (string[])
-parking_fee (string[])
-graceperiod (string[])</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"messagetype" : "Parkinglot_List",
-"parkinglot_count" : 3,
-"parkinglot_id" : ["1", "2", "3"],
-"parkinglot_location" : ["811 S Negley Pittsburgh", "b", "c"],
-"parking_fee" : ["5.99", "10.99", "15.99"],
-"graceperiod" : ["120", "30", "0"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">messagetype (string)
-parkinglot_count (int)
-parkinglot_id (string[])
-parkinglot_location (string[])
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>parking_fee</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (string[])
-graceperiod (string[])</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"messagetype" : "Parkinglot_List",
-"parkinglot_count" : 3,
-"parkinglot_id" : ["1", "2", "3"],
-"parkinglot_location" : ["811 S Negley Pittsburgh", "b", "c"],
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>parking_fee</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : ["5.99", "10.99", "15.99"],
-"graceperiod" : ["120", "30", "0"]</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -949,6 +867,196 @@
 graceperiod (string)
 paymentinfo (string)
 confirmationinfo (string)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">messagetype (string)
+parkinglot_count (int)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parkinglot_id_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (string[])
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parkinglot_location_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (string[])
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking_fee_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (string[])
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>graceperiod_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (string[])</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"messagetype" : "Parkinglot_List",
+"parkinglot_count" : 3,
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parkinglot_id_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : ["1", "2", "3"],
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parkinglot_location_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : ["811 S Negley Pittsburgh", "b", "c"],
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking_fee_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : ["5.99", "10.99", "15.99"],
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>graceperiod_list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : ["120", "30", "0"]</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2165,11 +2273,11 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2313,12 +2421,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2328,7 +2436,7 @@
     <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.75" customWidth="1"/>
     <col min="5" max="5" width="21.25" customWidth="1"/>
-    <col min="6" max="6" width="53.875" customWidth="1"/>
+    <col min="6" max="6" width="56.5" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2394,13 +2502,13 @@
         <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -2427,7 +2535,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2435,12 +2543,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2647,7 +2755,7 @@
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="B2:F6"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2703,13 +2811,13 @@
         <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="165">

</xml_diff>